<commit_message>
Ripristinata API mappings con database e migliorato logging file-info
</commit_message>
<xml_diff>
--- a/File temporanei/Export - 2025-08-29T082851.500.Xlsx
+++ b/File temporanei/Export - 2025-08-29T082851.500.Xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DB_Partesa\Import\File Delivery\Da importare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Progetti\Cursor\gestione-partesa\File temporanei\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F4DC77-ACBD-44B8-AC7D-E6E08823663B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9932BBF7-BA1D-4A0C-A24B-F9ED6A75B1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,7 +419,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,10 +476,10 @@
         <v>11</v>
       </c>
       <c r="D2" s="4">
-        <v>45897.2722222222</v>
+        <v>45900.272222222222</v>
       </c>
       <c r="E2" s="4">
-        <v>45897.516666666699</v>
+        <v>45900.51666666667</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
@@ -511,10 +511,10 @@
         <v>11</v>
       </c>
       <c r="D3" s="4">
-        <v>45897.309027777803</v>
+        <v>45900.272222222222</v>
       </c>
       <c r="E3" s="4">
-        <v>45897.441666666702</v>
+        <v>45900.51666666667</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>13</v>
@@ -546,10 +546,10 @@
         <v>11</v>
       </c>
       <c r="D4" s="4">
-        <v>45897.306250000001</v>
+        <v>45900.272222222222</v>
       </c>
       <c r="E4" s="4">
-        <v>45897.489583333299</v>
+        <v>45900.51666666667</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>14</v>
@@ -581,10 +581,10 @@
         <v>11</v>
       </c>
       <c r="D5" s="4">
-        <v>45897.320833333302</v>
+        <v>45900.272222222222</v>
       </c>
       <c r="E5" s="4">
-        <v>45897.581250000003</v>
+        <v>45900.51666666667</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>15</v>
@@ -616,10 +616,10 @@
         <v>11</v>
       </c>
       <c r="D6" s="4">
-        <v>45897.327083333301</v>
+        <v>45900.272222222222</v>
       </c>
       <c r="E6" s="4">
-        <v>45897.541666666701</v>
+        <v>45900.51666666667</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>16</v>

</xml_diff>